<commit_message>
Repairing the second walk starting time detection
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -178,9 +178,6 @@
     <t>3:40,</t>
   </si>
   <si>
-    <t>1008, 673, 1275, 673</t>
-  </si>
-  <si>
     <t>5:50,</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>4:45,</t>
+  </si>
+  <si>
+    <t>993, 630, 1260, 630</t>
   </si>
   <si>
     <t>9:06,</t>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
+      <selection activeCell="J441" sqref="J441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3508,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>75</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>75</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>76</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>76</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>76</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>77</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>77</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>77</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>78</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>78</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>78</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>79</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>79</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>79</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>80</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>80</v>
       </c>
@@ -3700,9 +3700,6 @@
       </c>
       <c r="F240">
         <v>3</v>
-      </c>
-      <c r="H240" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
@@ -3801,7 +3798,7 @@
         <v>22</v>
       </c>
       <c r="E246" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F246">
         <v>3</v>
@@ -4131,10 +4128,10 @@
         <v>1</v>
       </c>
       <c r="D273" t="s">
+        <v>55</v>
+      </c>
+      <c r="E273" t="s">
         <v>56</v>
-      </c>
-      <c r="E273" t="s">
-        <v>57</v>
       </c>
       <c r="F273">
         <v>1</v>
@@ -4209,7 +4206,7 @@
         <v>22</v>
       </c>
       <c r="E279" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F279">
         <v>3</v>
@@ -4515,7 +4512,7 @@
         <v>22</v>
       </c>
       <c r="E306" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F306">
         <v>3</v>
@@ -4692,7 +4689,7 @@
         <v>3</v>
       </c>
       <c r="G321" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
@@ -4987,7 +4984,7 @@
         <v>22</v>
       </c>
       <c r="E344" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F344">
         <v>3</v>
@@ -5007,7 +5004,7 @@
         <v>22</v>
       </c>
       <c r="E345" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F345">
         <v>3</v>
@@ -5170,7 +5167,7 @@
         <v>22</v>
       </c>
       <c r="E359" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F359">
         <v>3</v>
@@ -5283,7 +5280,7 @@
         <v>22</v>
       </c>
       <c r="E366" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F366">
         <v>3</v>
@@ -5314,7 +5311,7 @@
         <v>22</v>
       </c>
       <c r="E368" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F368">
         <v>3</v>
@@ -5557,7 +5554,7 @@
         <v>22</v>
       </c>
       <c r="E386" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F386">
         <v>3</v>
@@ -5577,7 +5574,7 @@
         <v>22</v>
       </c>
       <c r="E387" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F387">
         <v>3</v>
@@ -5641,7 +5638,7 @@
         <v>22</v>
       </c>
       <c r="E392" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F392">
         <v>3</v>
@@ -5664,7 +5661,7 @@
         <v>3</v>
       </c>
       <c r="G393" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.25">
@@ -5802,7 +5799,7 @@
         <v>22</v>
       </c>
       <c r="E405" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F405">
         <v>3</v>
@@ -5866,13 +5863,13 @@
         <v>22</v>
       </c>
       <c r="E410" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F410">
         <v>3</v>
       </c>
       <c r="G410" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.25">
@@ -6126,7 +6123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>144</v>
       </c>
@@ -6137,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>145</v>
       </c>
@@ -6148,7 +6145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>145</v>
       </c>
@@ -6159,7 +6156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>145</v>
       </c>
@@ -6170,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>146</v>
       </c>
@@ -6181,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>146</v>
       </c>
@@ -6192,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>146</v>
       </c>
@@ -6203,7 +6200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>147</v>
       </c>
@@ -6217,13 +6214,13 @@
         <v>22</v>
       </c>
       <c r="E440" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F440">
         <v>3</v>
       </c>
     </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>147</v>
       </c>
@@ -6242,8 +6239,11 @@
       <c r="F441">
         <v>3</v>
       </c>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H441" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>147</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>1001</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>1002</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>1003</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>1004</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>1005</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>1006</v>
       </c>

</xml_diff>

<commit_message>
person detection precision update
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -30,7 +30,7 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <b val="1"/>
       <color theme="1"/>
@@ -451,16 +451,16 @@
   </sheetPr>
   <dimension ref="A1:J490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
+      <selection activeCell="E259" sqref="E259"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
     <col width="10" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.4" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Number</t>
@@ -999,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="J26" t="n">
-        <v>1.375</v>
+        <v>1.212121212121212</v>
       </c>
     </row>
     <row r="27">
@@ -1230,11 +1230,16 @@
           <t>3/4,</t>
         </is>
       </c>
-      <c r="E38" s="3" t="n">
-        <v>0.2284722222222222</v>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>5:29,</t>
+        </is>
       </c>
       <c r="F38" t="n">
         <v>2</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1.165048543689321</v>
       </c>
     </row>
     <row r="39">
@@ -1358,6 +1363,19 @@
       <c r="F45" t="n">
         <v>1</v>
       </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>940, 431, 1206, 431</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>861, 755, 1195, 755</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
+        <v>1.20752427184466</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1525,7 +1543,7 @@
         </is>
       </c>
       <c r="J54" t="n">
-        <v>1.121739130434783</v>
+        <v>1.115798536375377</v>
       </c>
     </row>
     <row r="55">
@@ -1566,6 +1584,19 @@
       <c r="F56" t="n">
         <v>2</v>
       </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>1205, 533, 1471, 533</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>1148, 873, 1481, 873</t>
+        </is>
+      </c>
+      <c r="J56" t="n">
+        <v>0.8143172616856827</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1823,8 +1854,10 @@
           <t>1/4,</t>
         </is>
       </c>
-      <c r="E72" s="3" t="n">
-        <v>0.1875</v>
+      <c r="E72" s="3" t="inlineStr">
+        <is>
+          <t>4:30,</t>
+        </is>
       </c>
       <c r="F72" t="n">
         <v>1</v>
@@ -3259,6 +3292,19 @@
       <c r="F176" t="n">
         <v>3</v>
       </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>830, 600, 1096, 600</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>843, 986, 1176, 986</t>
+        </is>
+      </c>
+      <c r="J176" t="n">
+        <v>1.285909712722298</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -4161,6 +4207,19 @@
       <c r="F233" t="n">
         <v>3</v>
       </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>858, 650, 1125, 650</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>855, 985, 1188, 985</t>
+        </is>
+      </c>
+      <c r="J233" t="n">
+        <v>1.283026626914773</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -4271,7 +4330,7 @@
         </is>
       </c>
       <c r="J240" t="n">
-        <v>1.804613297150611</v>
+        <v>1.726708074534161</v>
       </c>
     </row>
     <row r="241">
@@ -4486,8 +4545,10 @@
           <t>1/4,</t>
         </is>
       </c>
-      <c r="E252" s="3" t="n">
-        <v>0.1458333333333333</v>
+      <c r="E252" s="3" t="inlineStr">
+        <is>
+          <t>3:30,</t>
+        </is>
       </c>
       <c r="F252" t="n">
         <v>3</v>
@@ -4575,8 +4636,10 @@
           <t>1/4,</t>
         </is>
       </c>
-      <c r="E258" s="3" t="n">
-        <v>0.2291666666666667</v>
+      <c r="E258" s="3" t="inlineStr">
+        <is>
+          <t>5:30,</t>
+        </is>
       </c>
       <c r="F258" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
Changing the GUI, so the speed will be shown after the video ends.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
passing line detection precision update, we fixed bugs when the foot coordinates disappeared we couldn't detect when the person passed the line, movement detection updated to be more precise.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -604,8 +604,8 @@
   </sheetPr>
   <dimension ref="A1:L1159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="O234" sqref="O234"/>
+    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
+      <selection activeCell="J360" sqref="J360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
@@ -1106,7 +1106,7 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>1.434634974533107</v>
+        <v>1.402173913043478</v>
       </c>
       <c r="K17" s="7" t="n">
         <v>1.33</v>
@@ -1166,7 +1166,7 @@
         </is>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
@@ -1195,9 +1195,6 @@
         <is>
           <t>988, 693, 1321, 693</t>
         </is>
-      </c>
-      <c r="J20" t="n">
-        <v>1.376923076923077</v>
       </c>
       <c r="K20" s="7" t="n">
         <v>1.07</v>
@@ -1226,7 +1223,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>3:50,</t>
+          <t>3:55,</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1241,6 +1238,9 @@
         <is>
           <t>1075, 1031, 1408, 1031</t>
         </is>
+      </c>
+      <c r="J21" t="n">
+        <v>1.106879918761107</v>
       </c>
       <c r="K21" s="8" t="n">
         <v>1.12</v>
@@ -1280,7 +1280,7 @@
         </is>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1340,16 +1340,16 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>931, 465, 1198, 465</t>
+          <t>928, 438, 1195, 438</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>908, 768, 1241, 768</t>
+          <t>893, 766, 1226, 766</t>
         </is>
       </c>
       <c r="J24" t="n">
-        <v>1.863442389758179</v>
+        <v>1.364341085271318</v>
       </c>
       <c r="K24" s="8" t="n">
         <v>1.36</v>
@@ -1407,7 +1407,7 @@
         <v>2</v>
       </c>
       <c r="J26" t="n">
-        <v>1.283714578354387</v>
+        <v>1.621621621621621</v>
       </c>
       <c r="K26" s="7" t="n">
         <v>1.4</v>
@@ -1452,9 +1452,6 @@
           <t>860, 773, 1193, 773</t>
         </is>
       </c>
-      <c r="J27" t="n">
-        <v>3.117408906882591</v>
-      </c>
       <c r="K27" s="8" t="n">
         <v>1.33</v>
       </c>
@@ -1555,7 +1552,7 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>1.327953044754219</v>
+        <v>1.47377938517179</v>
       </c>
       <c r="K30" s="8" t="n">
         <v>1.5</v>
@@ -1705,7 +1702,7 @@
         </is>
       </c>
       <c r="J36" t="n">
-        <v>1.087063453025086</v>
+        <v>1.13703405738804</v>
       </c>
       <c r="K36" s="8" t="n">
         <v>1.22</v>
@@ -1761,7 +1758,7 @@
         <v>2</v>
       </c>
       <c r="J38" t="n">
-        <v>1.165048543689321</v>
+        <v>1.512365250475586</v>
       </c>
       <c r="K38" s="7" t="n">
         <v>1.36</v>
@@ -1916,7 +1913,7 @@
         </is>
       </c>
       <c r="J44" t="n">
-        <v>1.428773919206237</v>
+        <v>1.610810810810811</v>
       </c>
       <c r="K44" s="7" t="n">
         <v>1.33</v>
@@ -1962,7 +1959,7 @@
         </is>
       </c>
       <c r="J45" t="n">
-        <v>1.20752427184466</v>
+        <v>1.260726072607261</v>
       </c>
       <c r="K45" s="8" t="n">
         <v>1.48</v>
@@ -2019,16 +2016,16 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1225, 541, 1491, 541</t>
+          <t>1223, 543, 1490, 543</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>1186, 880, 1520, 880</t>
+          <t>1163, 878, 1496, 878</t>
         </is>
       </c>
       <c r="J47" t="n">
-        <v>1.481707317073171</v>
+        <v>1.489655172413793</v>
       </c>
       <c r="K47" s="7" t="n">
         <v>1.1</v>
@@ -2217,7 +2214,7 @@
         </is>
       </c>
       <c r="J54" t="n">
-        <v>1.157699443413729</v>
+        <v>1.365554276946682</v>
       </c>
       <c r="K54" s="8" t="n">
         <v>1.39</v>
@@ -2283,7 +2280,7 @@
         </is>
       </c>
       <c r="J56" t="n">
-        <v>0.8326930464848252</v>
+        <v>0.8712121212121212</v>
       </c>
       <c r="K56" s="7" t="n">
         <v>0.89</v>
@@ -2328,6 +2325,9 @@
           <t>898, 1053, 1231, 1053</t>
         </is>
       </c>
+      <c r="J57" t="n">
+        <v>1.149362970994849</v>
+      </c>
       <c r="K57" s="8" t="n">
         <v>0.98</v>
       </c>
@@ -2403,16 +2403,16 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>978, 653, 1245, 653</t>
+          <t>973, 655, 1240, 655</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>913, 1053, 1246, 1053</t>
+          <t>883, 1053, 1216, 1053</t>
         </is>
       </c>
       <c r="J60" t="n">
-        <v>0.9283154121863799</v>
+        <v>0.9718032786885247</v>
       </c>
       <c r="K60" s="8" t="n">
         <v>1.14</v>
@@ -2629,7 +2629,7 @@
         </is>
       </c>
       <c r="J69" t="n">
-        <v>0.9876710472835659</v>
+        <v>1.057289240801118</v>
       </c>
       <c r="K69" s="8" t="n">
         <v>1.17</v>
@@ -2711,16 +2711,16 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>721, 541, 988, 541</t>
+          <t>728, 515, 995, 515</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>700, 975, 1033, 975</t>
+          <t>680, 976, 1013, 976</t>
         </is>
       </c>
       <c r="J72" t="n">
-        <v>1.36381247578458</v>
+        <v>1.174112256586483</v>
       </c>
       <c r="K72" s="8" t="n">
         <v>1.21</v>
@@ -3193,7 +3193,7 @@
         <v/>
       </c>
     </row>
-    <row r="91">
+    <row r="91" ht="13.2" customHeight="1">
       <c r="A91" t="n">
         <v>30</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>2</v>
       </c>
       <c r="J92" t="n">
-        <v>1.174112256586483</v>
+        <v>1.27891156462585</v>
       </c>
       <c r="K92" s="12" t="n">
         <v>1.67</v>
@@ -4811,7 +4811,7 @@
         </is>
       </c>
       <c r="J179" t="n">
-        <v>1.005046257359125</v>
+        <v>1.076774505070015</v>
       </c>
       <c r="K179" s="12" t="n">
         <v>1.38</v>
@@ -5234,7 +5234,7 @@
         </is>
       </c>
       <c r="J198" t="n">
-        <v>1.058275058275058</v>
+        <v>1.172098341909663</v>
       </c>
       <c r="K198" s="13" t="n">
         <v>0.92</v>
@@ -5313,11 +5313,16 @@
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>895, 630, 1161, 630</t>
+          <t>891, 585, 1158, 585</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>868, 933, 1201, 933</t>
         </is>
       </c>
       <c r="J201" t="n">
-        <v>1.847903340440654</v>
+        <v>1.320116054158607</v>
       </c>
       <c r="K201" s="13" t="n">
         <v>1.34</v>
@@ -5471,11 +5476,16 @@
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>891, 628, 1158, 628</t>
+          <t>898, 585, 1165, 585</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>865, 935, 1198, 935</t>
         </is>
       </c>
       <c r="J207" t="n">
-        <v>1.658263305322129</v>
+        <v>1.253446447507953</v>
       </c>
       <c r="K207" s="13" t="n">
         <v>1.16</v>
@@ -5800,16 +5810,16 @@
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>930, 556, 1196, 556</t>
+          <t>930, 560, 1196, 560</t>
         </is>
       </c>
       <c r="I221" t="inlineStr">
         <is>
-          <t>813, 1026, 1146, 1026</t>
+          <t>778, 1026, 1111, 1026</t>
         </is>
       </c>
       <c r="J221" t="n">
-        <v>1.380039656311963</v>
+        <v>1.206060606060606</v>
       </c>
       <c r="K221" s="12" t="n">
         <v>1</v>
@@ -6052,16 +6062,16 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>858, 650, 1125, 650</t>
+          <t>840, 600, 1106, 600</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>855, 985, 1188, 985</t>
+          <t>835, 990, 1168, 990</t>
         </is>
       </c>
       <c r="J233" t="n">
-        <v>2.071428571428571</v>
+        <v>1.392914653784219</v>
       </c>
       <c r="K233" s="12" t="n">
         <v>1.36</v>
@@ -6209,11 +6219,16 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>1008, 673, 1275, 673</t>
+          <t>991, 628, 1258, 628</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>961, 988, 1295, 988</t>
         </is>
       </c>
       <c r="J240" t="n">
-        <v>1.726708074534161</v>
+        <v>1.359447004608295</v>
       </c>
       <c r="K240" s="13" t="n">
         <v>1.38</v>
@@ -6270,11 +6285,16 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>876, 653, 1143, 653</t>
+          <t>896, 616, 1163, 616</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>806, 916, 1140, 916</t>
         </is>
       </c>
       <c r="J242" t="n">
-        <v>1.832167832167832</v>
+        <v>1.344180225281602</v>
       </c>
       <c r="K242" s="12" t="n">
         <v>1.33</v>
@@ -6331,16 +6351,16 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>753, 426, 1020, 426</t>
+          <t>753, 425, 1020, 425</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>770, 670, 1103, 670</t>
+          <t>760, 668, 1093, 668</t>
         </is>
       </c>
       <c r="J244" t="n">
-        <v>1.536203522504892</v>
+        <v>1.500465983224604</v>
       </c>
       <c r="K244" s="14" t="n">
         <v>1.34</v>
@@ -6423,11 +6443,16 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>875, 655, 1141, 655</t>
+          <t>905, 616, 1171, 616</t>
+        </is>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>813, 915, 1146, 915</t>
         </is>
       </c>
       <c r="J246" t="n">
-        <v>1.548451548451548</v>
+        <v>1.182294700058241</v>
       </c>
       <c r="K246" s="13" t="n">
         <v>1.09</v>
@@ -6564,11 +6589,16 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>896, 655, 1163, 655</t>
+          <t>900, 616, 1166, 616</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>810, 915, 1143, 915</t>
         </is>
       </c>
       <c r="J252" t="n">
-        <v>1.904761904761905</v>
+        <v>1.481481481481481</v>
       </c>
       <c r="K252" s="13" t="n">
         <v>1.36</v>
@@ -6709,16 +6739,16 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>808, 621, 1075, 621</t>
+          <t>816, 575, 1083, 575</t>
         </is>
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>753, 958, 1086, 958</t>
+          <t>741, 956, 1075, 956</t>
         </is>
       </c>
       <c r="J258" t="n">
-        <v>1.318840579710145</v>
+        <v>1.026841219922475</v>
       </c>
       <c r="K258" s="13" t="n">
         <v>1.06</v>
@@ -7167,16 +7197,16 @@
       </c>
       <c r="H279" t="inlineStr">
         <is>
-          <t>698, 705, 965, 705</t>
+          <t>706, 663, 973, 663</t>
         </is>
       </c>
       <c r="I279" t="inlineStr">
         <is>
-          <t>618, 976, 951, 976</t>
+          <t>600, 975, 933, 975</t>
         </is>
       </c>
       <c r="J279" t="n">
-        <v>1.455882352941176</v>
+        <v>1.107142857142857</v>
       </c>
       <c r="K279" s="13" t="n">
         <v>1.11</v>
@@ -8026,7 +8056,7 @@
         </is>
       </c>
       <c r="J322" t="n">
-        <v>1.090999256136871</v>
+        <v>1.18252427184466</v>
       </c>
       <c r="K322" s="14" t="n">
         <v>1.25</v>
@@ -8354,11 +8384,16 @@
       </c>
       <c r="H338" t="inlineStr">
         <is>
-          <t>816, 596, 1083, 596</t>
+          <t>803, 601, 1070, 601</t>
+        </is>
+      </c>
+      <c r="I338" t="inlineStr">
+        <is>
+          <t>830, 988, 1163, 988</t>
         </is>
       </c>
       <c r="J338" t="n">
-        <v>0.8181818181818181</v>
+        <v>0.9533417402269861</v>
       </c>
       <c r="K338" s="12" t="n">
         <v>1.33</v>
@@ -8395,13 +8430,16 @@
       </c>
       <c r="H339" t="inlineStr">
         <is>
-          <t>811, 565, 1078, 565</t>
+          <t>813, 558, 1080, 558</t>
         </is>
       </c>
       <c r="I339" t="inlineStr">
         <is>
-          <t>735, 881, 1068, 881</t>
-        </is>
+          <t>721, 881, 1055, 881</t>
+        </is>
+      </c>
+      <c r="J339" t="n">
+        <v>1.539473684210526</v>
       </c>
       <c r="K339" s="13" t="n">
         <v>1.51</v>
@@ -8462,7 +8500,7 @@
         </is>
       </c>
       <c r="J341" t="n">
-        <v>1.277173913043478</v>
+        <v>1.284340659340659</v>
       </c>
       <c r="K341" s="12" t="n">
         <v>1.13</v>
@@ -8548,7 +8586,7 @@
         </is>
       </c>
       <c r="J344" t="n">
-        <v>1.421362489486964</v>
+        <v>1.326331216414265</v>
       </c>
       <c r="K344" s="12" t="n">
         <v>1.26</v>
@@ -8923,7 +8961,7 @@
         </is>
       </c>
       <c r="J360" t="n">
-        <v>1.137078651685393</v>
+        <v>1.646616541353383</v>
       </c>
       <c r="K360" s="13" t="n">
         <v>1.33</v>
@@ -9173,6 +9211,9 @@
           <t>841, 990, 1175, 990</t>
         </is>
       </c>
+      <c r="J368" t="n">
+        <v>1.157699443413729</v>
+      </c>
       <c r="K368" s="12" t="n">
         <v>1.16</v>
       </c>
@@ -9208,16 +9249,16 @@
       </c>
       <c r="H369" t="inlineStr">
         <is>
-          <t>763, 558, 1030, 558</t>
+          <t>780, 560, 1046, 560</t>
         </is>
       </c>
       <c r="I369" t="inlineStr">
         <is>
-          <t>671, 881, 1005, 881</t>
+          <t>675, 883, 1008, 883</t>
         </is>
       </c>
       <c r="J369" t="n">
-        <v>1.266666666666667</v>
+        <v>1.20752427184466</v>
       </c>
       <c r="K369" s="13" t="n">
         <v>1.1</v>
@@ -9315,12 +9356,12 @@
       </c>
       <c r="H372" t="inlineStr">
         <is>
-          <t>903, 628, 1170, 628</t>
+          <t>935, 586, 1201, 586</t>
         </is>
       </c>
       <c r="I372" t="inlineStr">
         <is>
-          <t>955, 1003, 1288, 1003</t>
+          <t>936, 1001, 1270, 1001</t>
         </is>
       </c>
       <c r="K372" s="13" t="n">
@@ -9520,16 +9561,16 @@
       </c>
       <c r="H382" t="inlineStr">
         <is>
-          <t>761, 423, 1028, 423</t>
+          <t>753, 426, 1020, 426</t>
         </is>
       </c>
       <c r="I382" t="inlineStr">
         <is>
-          <t>758, 673, 1091, 673</t>
+          <t>760, 668, 1093, 668</t>
         </is>
       </c>
       <c r="J382" t="n">
-        <v>1.256578947368421</v>
+        <v>1.483516483516484</v>
       </c>
       <c r="K382" s="14" t="n">
         <v>1.47</v>
@@ -9789,7 +9830,7 @@
         </is>
       </c>
       <c r="J392" t="n">
-        <v>1.026315789473684</v>
+        <v>1.35258358662614</v>
       </c>
       <c r="K392" s="12" t="n">
         <v>1.26</v>
@@ -10052,16 +10093,16 @@
       </c>
       <c r="H405" t="inlineStr">
         <is>
-          <t>786, 560, 1053, 560</t>
+          <t>806, 538, 1073, 538</t>
         </is>
       </c>
       <c r="I405" t="inlineStr">
         <is>
-          <t>698, 880, 1031, 880</t>
+          <t>681, 883, 1015, 883</t>
         </is>
       </c>
       <c r="J405" t="n">
-        <v>2.036238136324418</v>
+        <v>1.832167832167832</v>
       </c>
       <c r="K405" s="13" t="n">
         <v>1.43</v>
@@ -10174,13 +10215,16 @@
       </c>
       <c r="H410" t="inlineStr">
         <is>
-          <t>855, 530, 1121, 530</t>
+          <t>851, 528, 1118, 528</t>
         </is>
       </c>
       <c r="I410" t="inlineStr">
         <is>
-          <t>805, 956, 1138, 956</t>
-        </is>
+          <t>803, 960, 1136, 960</t>
+        </is>
+      </c>
+      <c r="J410" t="n">
+        <v>1.195479777954005</v>
       </c>
       <c r="K410" s="12" t="n">
         <v>1.26</v>
@@ -10765,16 +10809,16 @@
       </c>
       <c r="H440" t="inlineStr">
         <is>
-          <t>801, 653, 1068, 653</t>
+          <t>813, 615, 1080, 615</t>
         </is>
       </c>
       <c r="I440" t="inlineStr">
         <is>
-          <t>778, 913, 1111, 913</t>
+          <t>755, 915, 1088, 915</t>
         </is>
       </c>
       <c r="J440" t="n">
-        <v>1.368052856587641</v>
+        <v>0.971675845790716</v>
       </c>
       <c r="K440" s="12" t="n">
         <v>1.05</v>
@@ -11050,8 +11094,18 @@
       <c r="F452" t="n">
         <v>6</v>
       </c>
+      <c r="H452" t="inlineStr">
+        <is>
+          <t>701, 523, 968, 523</t>
+        </is>
+      </c>
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>738, 930, 1071, 930</t>
+        </is>
+      </c>
       <c r="J452" t="n">
-        <v>1.240195039219843</v>
+        <v>1.411764705882353</v>
       </c>
       <c r="K452" s="23" t="n">
         <v>1.333333333333333</v>
@@ -11097,7 +11151,7 @@
         </is>
       </c>
       <c r="J453" t="n">
-        <v>1.212121212121212</v>
+        <v>1.057453416149068</v>
       </c>
       <c r="K453" s="23" t="n">
         <v>1.333333333333333</v>
@@ -11158,7 +11212,7 @@
         </is>
       </c>
       <c r="J455" t="n">
-        <v>0.8770806658130601</v>
+        <v>0.8451123344740366</v>
       </c>
       <c r="K455" s="23" t="n">
         <v>1</v>
@@ -11204,7 +11258,7 @@
         </is>
       </c>
       <c r="J456" t="n">
-        <v>1.218211648892535</v>
+        <v>1.196428571428571</v>
       </c>
       <c r="K456" s="23" t="n">
         <v>1.129943502824859</v>
@@ -11250,7 +11304,7 @@
         </is>
       </c>
       <c r="J457" t="n">
-        <v>0.7920878354827466</v>
+        <v>0.8637116818558409</v>
       </c>
       <c r="K457" s="23" t="n">
         <v>1</v>
@@ -11287,16 +11341,16 @@
       </c>
       <c r="H458" t="inlineStr">
         <is>
-          <t>450, 243, 716, 243</t>
+          <t>435, 243, 701, 243</t>
         </is>
       </c>
       <c r="I458" t="inlineStr">
         <is>
-          <t>361, 441, 695, 441</t>
+          <t>350, 441, 683, 441</t>
         </is>
       </c>
       <c r="J458" t="n">
-        <v>1.162552398695855</v>
+        <v>1.285909712722298</v>
       </c>
       <c r="K458" s="23" t="n">
         <v>1.333333333333333</v>
@@ -11342,7 +11396,7 @@
         </is>
       </c>
       <c r="J459" t="n">
-        <v>1.246233318984072</v>
+        <v>1.191037735849056</v>
       </c>
       <c r="K459" s="23" t="n">
         <v>1.066666666666667</v>
@@ -11377,8 +11431,18 @@
       <c r="F460" t="n">
         <v>6</v>
       </c>
+      <c r="H460" t="inlineStr">
+        <is>
+          <t>735, 521, 1001, 521</t>
+        </is>
+      </c>
+      <c r="I460" t="inlineStr">
+        <is>
+          <t>768, 925, 1101, 925</t>
+        </is>
+      </c>
       <c r="J460" t="n">
-        <v>1.03725782414307</v>
+        <v>1.15045871559633</v>
       </c>
       <c r="K460" s="23" t="n">
         <v>1.081081081081081</v>
@@ -11424,7 +11488,7 @@
         </is>
       </c>
       <c r="J461" t="n">
-        <v>0.8909589041095891</v>
+        <v>0.9674922600619195</v>
       </c>
       <c r="K461" s="23" t="n">
         <v>1.142857142857143</v>
@@ -11502,8 +11566,18 @@
       <c r="F463" t="n">
         <v>5</v>
       </c>
+      <c r="H463" t="inlineStr">
+        <is>
+          <t>773, 506, 1040, 506</t>
+        </is>
+      </c>
+      <c r="I463" t="inlineStr">
+        <is>
+          <t>743, 710, 1076, 710</t>
+        </is>
+      </c>
       <c r="J463" t="n">
-        <v>1.579220779220779</v>
+        <v>1.920122887864823</v>
       </c>
       <c r="K463" s="23" t="n">
         <v>2.105263157894737</v>
@@ -11538,8 +11612,13 @@
       <c r="F464" t="n">
         <v>5</v>
       </c>
+      <c r="H464" t="inlineStr">
+        <is>
+          <t>761, 505, 1028, 505</t>
+        </is>
+      </c>
       <c r="J464" t="n">
-        <v>1.420168067226891</v>
+        <v>1.621917808219178</v>
       </c>
       <c r="K464" s="23" t="n">
         <v>1.616161616161616</v>
@@ -11590,7 +11669,7 @@
         </is>
       </c>
       <c r="J465" t="n">
-        <v>1.191037735849056</v>
+        <v>1.081124757595346</v>
       </c>
       <c r="K465" s="23" t="n">
         <v>1.095890410958904</v>
@@ -11625,8 +11704,18 @@
       <c r="F466" t="n">
         <v>5</v>
       </c>
+      <c r="H466" t="inlineStr">
+        <is>
+          <t>770, 505, 1036, 505</t>
+        </is>
+      </c>
+      <c r="I466" t="inlineStr">
+        <is>
+          <t>773, 710, 1106, 710</t>
+        </is>
+      </c>
       <c r="J466" t="n">
-        <v>1.512365250475586</v>
+        <v>1.693163751987281</v>
       </c>
       <c r="K466" s="23" t="n">
         <v>1.904761904761905</v>
@@ -11661,8 +11750,18 @@
       <c r="F467" t="n">
         <v>5</v>
       </c>
+      <c r="H467" t="inlineStr">
+        <is>
+          <t>780, 478, 1046, 478</t>
+        </is>
+      </c>
+      <c r="I467" t="inlineStr">
+        <is>
+          <t>758, 683, 1091, 683</t>
+        </is>
+      </c>
       <c r="J467" t="n">
-        <v>1.272727272727273</v>
+        <v>1.420565984869711</v>
       </c>
       <c r="K467" s="23" t="n">
         <v>1.379310344827586</v>
@@ -11728,7 +11827,7 @@
         </is>
       </c>
       <c r="J469" t="n">
-        <v>1.29091960670908</v>
+        <v>1.176923076923077</v>
       </c>
       <c r="K469" s="23" t="n">
         <v>1.176470588235294</v>
@@ -11763,8 +11862,15 @@
       <c r="F470" t="n">
         <v>5</v>
       </c>
-      <c r="J470" t="n">
-        <v>1.204335608189482</v>
+      <c r="H470" t="inlineStr">
+        <is>
+          <t>770, 478, 1036, 478</t>
+        </is>
+      </c>
+      <c r="I470" t="inlineStr">
+        <is>
+          <t>775, 683, 1108, 683</t>
+        </is>
       </c>
       <c r="K470" s="23" t="n">
         <v>1.151079136690647</v>
@@ -11799,8 +11905,18 @@
       <c r="F471" t="n">
         <v>5</v>
       </c>
+      <c r="H471" t="inlineStr">
+        <is>
+          <t>763, 478, 1030, 478</t>
+        </is>
+      </c>
+      <c r="I471" t="inlineStr">
+        <is>
+          <t>761, 681, 1095, 681</t>
+        </is>
+      </c>
       <c r="J471" t="n">
-        <v>1.106578276389597</v>
+        <v>1.256578947368421</v>
       </c>
       <c r="K471" s="23" t="n">
         <v>0.5333333333333333</v>
@@ -11835,8 +11951,18 @@
       <c r="F472" t="n">
         <v>6</v>
       </c>
+      <c r="H472" t="inlineStr">
+        <is>
+          <t>845, 551, 1111, 551</t>
+        </is>
+      </c>
+      <c r="I472" t="inlineStr">
+        <is>
+          <t>1006, 980, 1340, 980</t>
+        </is>
+      </c>
       <c r="J472" t="n">
-        <v>1.289655172413793</v>
+        <v>1.025715955581531</v>
       </c>
       <c r="K472" s="23" t="n">
         <v>1.081081081081081</v>
@@ -11914,8 +12040,18 @@
       <c r="F474" t="n">
         <v>6</v>
       </c>
+      <c r="H474" t="inlineStr">
+        <is>
+          <t>836, 551, 1103, 551</t>
+        </is>
+      </c>
+      <c r="I474" t="inlineStr">
+        <is>
+          <t>1048, 976, 1381, 976</t>
+        </is>
+      </c>
       <c r="J474" t="n">
-        <v>1.184594436879984</v>
+        <v>1.015574994666098</v>
       </c>
       <c r="K474" s="23" t="n">
         <v>1.038961038961039</v>
@@ -11950,8 +12086,18 @@
       <c r="F475" t="n">
         <v>6</v>
       </c>
+      <c r="H475" t="inlineStr">
+        <is>
+          <t>845, 551, 1111, 551</t>
+        </is>
+      </c>
+      <c r="I475" t="inlineStr">
+        <is>
+          <t>1016, 976, 1350, 976</t>
+        </is>
+      </c>
       <c r="J475" t="n">
-        <v>1.404709748083242</v>
+        <v>1.18252427184466</v>
       </c>
       <c r="K475" s="23" t="n">
         <v>1.13960113960114</v>
@@ -11986,8 +12132,13 @@
       <c r="F476" t="n">
         <v>5</v>
       </c>
+      <c r="H476" t="inlineStr">
+        <is>
+          <t>773, 480, 1040, 480</t>
+        </is>
+      </c>
       <c r="J476" t="n">
-        <v>1.04735883424408</v>
+        <v>1.233396584440228</v>
       </c>
       <c r="K476" s="23" t="n">
         <v>1.012658227848101</v>
@@ -12042,8 +12193,18 @@
       <c r="F478" t="n">
         <v>5</v>
       </c>
+      <c r="H478" t="inlineStr">
+        <is>
+          <t>756, 400, 1023, 400</t>
+        </is>
+      </c>
+      <c r="I478" t="inlineStr">
+        <is>
+          <t>631, 596, 965, 596</t>
+        </is>
+      </c>
       <c r="J478" t="n">
-        <v>1.194769169803844</v>
+        <v>1.333497962711446</v>
       </c>
       <c r="K478" s="23" t="n">
         <v>1.333333333333333</v>
@@ -12078,8 +12239,18 @@
       <c r="F479" t="n">
         <v>6</v>
       </c>
+      <c r="H479" t="inlineStr">
+        <is>
+          <t>756, 493, 1023, 493</t>
+        </is>
+      </c>
+      <c r="I479" t="inlineStr">
+        <is>
+          <t>548, 760, 881, 760</t>
+        </is>
+      </c>
       <c r="J479" t="n">
-        <v>1.144518121536924</v>
+        <v>1.206060606060606</v>
       </c>
       <c r="K479" s="23" t="n">
         <v>1.538461538461538</v>
@@ -12115,7 +12286,7 @@
         <v>6</v>
       </c>
       <c r="J480" t="n">
-        <v>0.952921157118548</v>
+        <v>1.00250626566416</v>
       </c>
       <c r="K480" s="23" t="n">
         <v>1.142857142857143</v>
@@ -12150,8 +12321,18 @@
       <c r="F481" t="n">
         <v>5</v>
       </c>
+      <c r="H481" t="inlineStr">
+        <is>
+          <t>758, 400, 1025, 400</t>
+        </is>
+      </c>
+      <c r="I481" t="inlineStr">
+        <is>
+          <t>636, 598, 970, 598</t>
+        </is>
+      </c>
       <c r="J481" t="n">
-        <v>0.9639953542392568</v>
+        <v>1.086173001310616</v>
       </c>
       <c r="K481" s="23" t="n">
         <v>1.111111111111111</v>
@@ -12186,8 +12367,18 @@
       <c r="F482" t="n">
         <v>6</v>
       </c>
+      <c r="H482" t="inlineStr">
+        <is>
+          <t>741, 495, 1008, 495</t>
+        </is>
+      </c>
+      <c r="I482" t="inlineStr">
+        <is>
+          <t>540, 761, 873, 761</t>
+        </is>
+      </c>
       <c r="J482" t="n">
-        <v>1.188235294117647</v>
+        <v>1.084103062712688</v>
       </c>
       <c r="K482" s="23" t="n">
         <v>1.24031007751938</v>
@@ -12222,8 +12413,18 @@
       <c r="F483" t="n">
         <v>6</v>
       </c>
+      <c r="H483" t="inlineStr">
+        <is>
+          <t>746, 495, 1013, 495</t>
+        </is>
+      </c>
+      <c r="I483" t="inlineStr">
+        <is>
+          <t>556, 761, 890, 761</t>
+        </is>
+      </c>
       <c r="J483" t="n">
-        <v>1.245161290322581</v>
+        <v>1.304964539007092</v>
       </c>
       <c r="K483" s="23" t="n">
         <v>1.290322580645161</v>
@@ -12258,8 +12459,13 @@
       <c r="F484" t="n">
         <v>5</v>
       </c>
+      <c r="H484" t="inlineStr">
+        <is>
+          <t>761, 400, 1028, 400</t>
+        </is>
+      </c>
       <c r="J484" t="n">
-        <v>1.225638353309015</v>
+        <v>1.502112345485839</v>
       </c>
       <c r="K484" s="23" t="n">
         <v>1.428571428571429</v>
@@ -12294,8 +12500,13 @@
       <c r="F485" t="n">
         <v>6</v>
       </c>
+      <c r="H485" t="inlineStr">
+        <is>
+          <t>756, 400, 1023, 400</t>
+        </is>
+      </c>
       <c r="J485" t="n">
-        <v>0.9762845849802371</v>
+        <v>1.15045871559633</v>
       </c>
       <c r="K485" s="23" t="n">
         <v>1.025641025641026</v>
@@ -12341,7 +12552,7 @@
         </is>
       </c>
       <c r="J486" t="n">
-        <v>1.079903147699758</v>
+        <v>1.122377622377623</v>
       </c>
       <c r="K486" s="23" t="n">
         <v>1</v>
@@ -12370,14 +12581,19 @@
       </c>
       <c r="E487" t="inlineStr">
         <is>
-          <t>8:57,</t>
+          <t>8:30,</t>
         </is>
       </c>
       <c r="F487" t="n">
         <v>5</v>
       </c>
+      <c r="H487" t="inlineStr">
+        <is>
+          <t>776, 401, 1043, 401</t>
+        </is>
+      </c>
       <c r="J487" t="n">
-        <v>0.8901098901098901</v>
+        <v>0.9880726484142044</v>
       </c>
       <c r="K487" s="23" t="n">
         <v>1</v>
@@ -12412,8 +12628,13 @@
       <c r="F488" t="n">
         <v>5</v>
       </c>
+      <c r="H488" t="inlineStr">
+        <is>
+          <t>751, 400, 1018, 400</t>
+        </is>
+      </c>
       <c r="J488" t="n">
-        <v>1.263297872340426</v>
+        <v>1.414898044111527</v>
       </c>
       <c r="K488" s="23" t="n">
         <v>1.403508771929824</v>
@@ -12448,8 +12669,18 @@
       <c r="F489" t="n">
         <v>6</v>
       </c>
+      <c r="H489" t="inlineStr">
+        <is>
+          <t>790, 431, 1056, 431</t>
+        </is>
+      </c>
+      <c r="I489" t="inlineStr">
+        <is>
+          <t>600, 695, 933, 695</t>
+        </is>
+      </c>
       <c r="J489" t="n">
-        <v>1.153952843273232</v>
+        <v>1.283459162663006</v>
       </c>
       <c r="K489" s="23" t="n">
         <v>1.324503311258278</v>
@@ -12485,7 +12716,7 @@
         <v>6</v>
       </c>
       <c r="J490" t="n">
-        <v>1.247575953458306</v>
+        <v>1.249190938511327</v>
       </c>
       <c r="K490" s="23" t="n">
         <v>1.111111111111111</v>

</xml_diff>